<commit_message>
Updated PairCorrelation tool to caluclate impermanent loss for Defi liquidity provision in AMM's.
</commit_message>
<xml_diff>
--- a/NetLiquidity/FRED_Data/WALCL.xlsx
+++ b/NetLiquidity/FRED_Data/WALCL.xlsx
@@ -434,7 +434,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B132"/>
+  <dimension ref="A1:B93"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,1050 +456,738 @@
     </row>
     <row r="2">
       <c r="A2" s="3" t="n">
-        <v>44048</v>
+        <v>44475</v>
       </c>
       <c r="B2" t="n">
-        <v>6945.237</v>
+        <v>8464.031999999999</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="n">
-        <v>44055</v>
+        <v>44482</v>
       </c>
       <c r="B3" t="n">
-        <v>6957.277</v>
+        <v>8480.941999999999</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="n">
-        <v>44062</v>
+        <v>44489</v>
       </c>
       <c r="B4" t="n">
-        <v>7010.637</v>
+        <v>8564.942999999999</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="n">
-        <v>44069</v>
+        <v>44496</v>
       </c>
       <c r="B5" t="n">
-        <v>6990.418</v>
+        <v>8556.181</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="n">
-        <v>44076</v>
+        <v>44503</v>
       </c>
       <c r="B6" t="n">
-        <v>7017.492</v>
+        <v>8574.870999999999</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="n">
-        <v>44083</v>
+        <v>44510</v>
       </c>
       <c r="B7" t="n">
-        <v>7010.614</v>
+        <v>8663.117</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="n">
-        <v>44090</v>
+        <v>44517</v>
       </c>
       <c r="B8" t="n">
-        <v>7064.475</v>
+        <v>8674.969999999999</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="n">
-        <v>44097</v>
+        <v>44524</v>
       </c>
       <c r="B9" t="n">
-        <v>7093.161</v>
+        <v>8681.771000000001</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="n">
-        <v>44104</v>
+        <v>44531</v>
       </c>
       <c r="B10" t="n">
-        <v>7056.129</v>
+        <v>8650.402</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="n">
-        <v>44111</v>
+        <v>44538</v>
       </c>
       <c r="B11" t="n">
-        <v>7074.649</v>
+        <v>8664.523999999999</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="3" t="n">
-        <v>44118</v>
+        <v>44545</v>
       </c>
       <c r="B12" t="n">
-        <v>7151.426</v>
+        <v>8756.665999999999</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="3" t="n">
-        <v>44125</v>
+        <v>44552</v>
       </c>
       <c r="B13" t="n">
-        <v>7177.265</v>
+        <v>8790.495000000001</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="3" t="n">
-        <v>44132</v>
+        <v>44559</v>
       </c>
       <c r="B14" t="n">
-        <v>7146.306</v>
+        <v>8757.459999999999</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="3" t="n">
-        <v>44139</v>
+        <v>44566</v>
       </c>
       <c r="B15" t="n">
-        <v>7157.479</v>
+        <v>8765.721</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="3" t="n">
-        <v>44146</v>
+        <v>44573</v>
       </c>
       <c r="B16" t="n">
-        <v>7175.417</v>
+        <v>8788.278</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="3" t="n">
-        <v>44153</v>
+        <v>44580</v>
       </c>
       <c r="B17" t="n">
-        <v>7243.08</v>
+        <v>8867.834000000001</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="3" t="n">
-        <v>44160</v>
+        <v>44587</v>
       </c>
       <c r="B18" t="n">
-        <v>7216.48</v>
+        <v>8860.485000000001</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="3" t="n">
-        <v>44167</v>
+        <v>44594</v>
       </c>
       <c r="B19" t="n">
-        <v>7222.414</v>
+        <v>8873.210999999999</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="3" t="n">
-        <v>44174</v>
+        <v>44601</v>
       </c>
       <c r="B20" t="n">
-        <v>7242.658</v>
+        <v>8878.009</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="3" t="n">
-        <v>44181</v>
+        <v>44608</v>
       </c>
       <c r="B21" t="n">
-        <v>7362.592</v>
+        <v>8911.032999999999</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="3" t="n">
-        <v>44188</v>
+        <v>44615</v>
       </c>
       <c r="B22" t="n">
-        <v>7404.039</v>
+        <v>8928.129000000001</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="3" t="n">
-        <v>44195</v>
+        <v>44622</v>
       </c>
       <c r="B23" t="n">
-        <v>7363.351</v>
+        <v>8904.455</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="3" t="n">
-        <v>44202</v>
+        <v>44629</v>
       </c>
       <c r="B24" t="n">
-        <v>7334.809</v>
+        <v>8910.748</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="3" t="n">
-        <v>44209</v>
+        <v>44636</v>
       </c>
       <c r="B25" t="n">
-        <v>7333.968</v>
+        <v>8954.306</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="3" t="n">
-        <v>44216</v>
+        <v>44643</v>
       </c>
       <c r="B26" t="n">
-        <v>7414.942</v>
+        <v>8962.474</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="3" t="n">
-        <v>44223</v>
+        <v>44650</v>
       </c>
       <c r="B27" t="n">
-        <v>7404.926</v>
+        <v>8937.142</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="3" t="n">
-        <v>44230</v>
+        <v>44657</v>
       </c>
       <c r="B28" t="n">
-        <v>7410.598</v>
+        <v>8937.592000000001</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="3" t="n">
-        <v>44237</v>
+        <v>44664</v>
       </c>
       <c r="B29" t="n">
-        <v>7442.225</v>
+        <v>8965.486999999999</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="3" t="n">
-        <v>44244</v>
+        <v>44671</v>
       </c>
       <c r="B30" t="n">
-        <v>7557.402</v>
+        <v>8955.851000000001</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="3" t="n">
-        <v>44251</v>
+        <v>44678</v>
       </c>
       <c r="B31" t="n">
-        <v>7590.111</v>
+        <v>8939.199000000001</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="3" t="n">
-        <v>44258</v>
+        <v>44685</v>
       </c>
       <c r="B32" t="n">
-        <v>7557.524</v>
+        <v>8939.972</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="3" t="n">
-        <v>44265</v>
+        <v>44692</v>
       </c>
       <c r="B33" t="n">
-        <v>7579.901</v>
+        <v>8942.008</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="3" t="n">
-        <v>44272</v>
+        <v>44699</v>
       </c>
       <c r="B34" t="n">
-        <v>7693.506</v>
+        <v>8945.897999999999</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="3" t="n">
-        <v>44279</v>
+        <v>44706</v>
       </c>
       <c r="B35" t="n">
-        <v>7719.622</v>
+        <v>8914.281000000001</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="3" t="n">
-        <v>44286</v>
+        <v>44713</v>
       </c>
       <c r="B36" t="n">
-        <v>7688.988</v>
+        <v>8915.049999999999</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="3" t="n">
-        <v>44293</v>
+        <v>44720</v>
       </c>
       <c r="B37" t="n">
-        <v>7708.882</v>
+        <v>8918.254000000001</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="3" t="n">
-        <v>44300</v>
+        <v>44727</v>
       </c>
       <c r="B38" t="n">
-        <v>7793.104</v>
+        <v>8932.42</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="3" t="n">
-        <v>44307</v>
+        <v>44734</v>
       </c>
       <c r="B39" t="n">
-        <v>7820.948</v>
+        <v>8934.346</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="3" t="n">
-        <v>44314</v>
+        <v>44741</v>
       </c>
       <c r="B40" t="n">
-        <v>7780.962</v>
+        <v>8913.553</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="3" t="n">
-        <v>44321</v>
+        <v>44748</v>
       </c>
       <c r="B41" t="n">
-        <v>7810.486</v>
+        <v>8891.851000000001</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="3" t="n">
-        <v>44328</v>
+        <v>44755</v>
       </c>
       <c r="B42" t="n">
-        <v>7830.663</v>
+        <v>8895.867</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="3" t="n">
-        <v>44335</v>
+        <v>44762</v>
       </c>
       <c r="B43" t="n">
-        <v>7922.883</v>
+        <v>8899.213</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="3" t="n">
-        <v>44342</v>
+        <v>44769</v>
       </c>
       <c r="B44" t="n">
-        <v>7903.541</v>
+        <v>8890.004000000001</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="3" t="n">
-        <v>44349</v>
+        <v>44776</v>
       </c>
       <c r="B45" t="n">
-        <v>7935.703</v>
+        <v>8874.620000000001</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="3" t="n">
-        <v>44356</v>
+        <v>44783</v>
       </c>
       <c r="B46" t="n">
-        <v>7952.327</v>
+        <v>8879.138000000001</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="3" t="n">
-        <v>44363</v>
+        <v>44790</v>
       </c>
       <c r="B47" t="n">
-        <v>8064.257</v>
+        <v>8849.762000000001</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="3" t="n">
-        <v>44370</v>
+        <v>44797</v>
       </c>
       <c r="B48" t="n">
-        <v>8101.945</v>
+        <v>8851.436</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="3" t="n">
-        <v>44377</v>
+        <v>44804</v>
       </c>
       <c r="B49" t="n">
-        <v>8078.544</v>
+        <v>8826.093000000001</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="3" t="n">
-        <v>44384</v>
+        <v>44811</v>
       </c>
       <c r="B50" t="n">
-        <v>8097.773</v>
+        <v>8822.401</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="3" t="n">
-        <v>44391</v>
+        <v>44818</v>
       </c>
       <c r="B51" t="n">
-        <v>8201.651</v>
+        <v>8832.759</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="3" t="n">
-        <v>44398</v>
+        <v>44825</v>
       </c>
       <c r="B52" t="n">
-        <v>8240.530000000001</v>
+        <v>8816.802</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="3" t="n">
-        <v>44405</v>
+        <v>44832</v>
       </c>
       <c r="B53" t="n">
-        <v>8221.473</v>
+        <v>8795.566999999999</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="3" t="n">
-        <v>44412</v>
+        <v>44839</v>
       </c>
       <c r="B54" t="n">
-        <v>8235.073</v>
+        <v>8759.053</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="3" t="n">
-        <v>44419</v>
+        <v>44846</v>
       </c>
       <c r="B55" t="n">
-        <v>8257.159</v>
+        <v>8758.968999999999</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="3" t="n">
-        <v>44426</v>
+        <v>44853</v>
       </c>
       <c r="B56" t="n">
-        <v>8342.598</v>
+        <v>8743.922</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="3" t="n">
-        <v>44433</v>
+        <v>44860</v>
       </c>
       <c r="B57" t="n">
-        <v>8332.743</v>
+        <v>8723.09</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="3" t="n">
-        <v>44440</v>
+        <v>44867</v>
       </c>
       <c r="B58" t="n">
-        <v>8349.173000000001</v>
+        <v>8676.870000000001</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="3" t="n">
-        <v>44447</v>
+        <v>44874</v>
       </c>
       <c r="B59" t="n">
-        <v>8357.314</v>
+        <v>8678.886</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="3" t="n">
-        <v>44454</v>
+        <v>44881</v>
       </c>
       <c r="B60" t="n">
-        <v>8448.77</v>
+        <v>8625.620000000001</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="3" t="n">
-        <v>44461</v>
+        <v>44888</v>
       </c>
       <c r="B61" t="n">
-        <v>8489.824000000001</v>
+        <v>8621.389999999999</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="3" t="n">
-        <v>44468</v>
+        <v>44895</v>
       </c>
       <c r="B62" t="n">
-        <v>8447.981</v>
+        <v>8584.575999999999</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="3" t="n">
-        <v>44475</v>
+        <v>44902</v>
       </c>
       <c r="B63" t="n">
-        <v>8464.031999999999</v>
+        <v>8582.735000000001</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="3" t="n">
-        <v>44482</v>
+        <v>44909</v>
       </c>
       <c r="B64" t="n">
-        <v>8480.941999999999</v>
+        <v>8583.413</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="3" t="n">
-        <v>44489</v>
+        <v>44916</v>
       </c>
       <c r="B65" t="n">
-        <v>8564.942999999999</v>
+        <v>8564.411</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="3" t="n">
-        <v>44496</v>
+        <v>44923</v>
       </c>
       <c r="B66" t="n">
-        <v>8556.181</v>
+        <v>8551.169</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="3" t="n">
-        <v>44503</v>
+        <v>44930</v>
       </c>
       <c r="B67" t="n">
-        <v>8574.870999999999</v>
+        <v>8507.429</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="3" t="n">
-        <v>44510</v>
+        <v>44937</v>
       </c>
       <c r="B68" t="n">
-        <v>8663.117</v>
+        <v>8508.587</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="3" t="n">
-        <v>44517</v>
+        <v>44944</v>
       </c>
       <c r="B69" t="n">
-        <v>8674.969999999999</v>
+        <v>8489.039000000001</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="3" t="n">
-        <v>44524</v>
+        <v>44951</v>
       </c>
       <c r="B70" t="n">
-        <v>8681.771000000001</v>
+        <v>8470.557000000001</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="3" t="n">
-        <v>44531</v>
+        <v>44958</v>
       </c>
       <c r="B71" t="n">
-        <v>8650.402</v>
+        <v>8433.610000000001</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="3" t="n">
-        <v>44538</v>
+        <v>44965</v>
       </c>
       <c r="B72" t="n">
-        <v>8664.523999999999</v>
+        <v>8435.369000000001</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="3" t="n">
-        <v>44545</v>
+        <v>44972</v>
       </c>
       <c r="B73" t="n">
-        <v>8756.665999999999</v>
+        <v>8384.767</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="3" t="n">
-        <v>44552</v>
+        <v>44979</v>
       </c>
       <c r="B74" t="n">
-        <v>8790.495000000001</v>
+        <v>8382.190000000001</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="3" t="n">
-        <v>44559</v>
+        <v>44986</v>
       </c>
       <c r="B75" t="n">
-        <v>8757.459999999999</v>
+        <v>8339.683999999999</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="3" t="n">
-        <v>44566</v>
+        <v>44993</v>
       </c>
       <c r="B76" t="n">
-        <v>8765.721</v>
+        <v>8342.282999999999</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="3" t="n">
-        <v>44573</v>
+        <v>45000</v>
       </c>
       <c r="B77" t="n">
-        <v>8788.278</v>
+        <v>8639.299999999999</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="3" t="n">
-        <v>44580</v>
+        <v>45007</v>
       </c>
       <c r="B78" t="n">
-        <v>8867.834000000001</v>
+        <v>8733.787</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="3" t="n">
-        <v>44587</v>
+        <v>45014</v>
       </c>
       <c r="B79" t="n">
-        <v>8860.485000000001</v>
+        <v>8705.941999999999</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="3" t="n">
-        <v>44594</v>
+        <v>45021</v>
       </c>
       <c r="B80" t="n">
-        <v>8873.210999999999</v>
+        <v>8632.384</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="3" t="n">
-        <v>44601</v>
+        <v>45028</v>
       </c>
       <c r="B81" t="n">
-        <v>8878.009</v>
+        <v>8614.797</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="3" t="n">
-        <v>44608</v>
+        <v>45035</v>
       </c>
       <c r="B82" t="n">
-        <v>8911.032999999999</v>
+        <v>8593.263000000001</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="3" t="n">
-        <v>44615</v>
+        <v>45042</v>
       </c>
       <c r="B83" t="n">
-        <v>8928.129000000001</v>
+        <v>8562.768</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="3" t="n">
-        <v>44622</v>
+        <v>45049</v>
       </c>
       <c r="B84" t="n">
-        <v>8904.455</v>
+        <v>8503.994000000001</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="3" t="n">
-        <v>44629</v>
+        <v>45056</v>
       </c>
       <c r="B85" t="n">
-        <v>8910.748</v>
+        <v>8503.017</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="3" t="n">
-        <v>44636</v>
+        <v>45063</v>
       </c>
       <c r="B86" t="n">
-        <v>8954.306</v>
+        <v>8456.76</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="3" t="n">
-        <v>44643</v>
+        <v>45070</v>
       </c>
       <c r="B87" t="n">
-        <v>8962.474</v>
+        <v>8436.254999999999</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="3" t="n">
-        <v>44650</v>
+        <v>45077</v>
       </c>
       <c r="B88" t="n">
-        <v>8937.142</v>
+        <v>8385.853999999999</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="3" t="n">
-        <v>44657</v>
+        <v>45084</v>
       </c>
       <c r="B89" t="n">
-        <v>8937.592000000001</v>
+        <v>8389.325000000001</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="3" t="n">
-        <v>44664</v>
+        <v>45091</v>
       </c>
       <c r="B90" t="n">
-        <v>8965.486999999999</v>
+        <v>8388.323</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="3" t="n">
-        <v>44671</v>
+        <v>45098</v>
       </c>
       <c r="B91" t="n">
-        <v>8955.851000000001</v>
+        <v>8362.059999999999</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="3" t="n">
-        <v>44678</v>
+        <v>45105</v>
       </c>
       <c r="B92" t="n">
-        <v>8939.199000000001</v>
+        <v>8340.914000000001</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="3" t="n">
-        <v>44685</v>
+        <v>45112</v>
       </c>
       <c r="B93" t="n">
-        <v>8939.972</v>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" s="3" t="n">
-        <v>44692</v>
-      </c>
-      <c r="B94" t="n">
-        <v>8942.008</v>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" s="3" t="n">
-        <v>44699</v>
-      </c>
-      <c r="B95" t="n">
-        <v>8945.897999999999</v>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" s="3" t="n">
-        <v>44706</v>
-      </c>
-      <c r="B96" t="n">
-        <v>8914.281000000001</v>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" s="3" t="n">
-        <v>44713</v>
-      </c>
-      <c r="B97" t="n">
-        <v>8915.049999999999</v>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" s="3" t="n">
-        <v>44720</v>
-      </c>
-      <c r="B98" t="n">
-        <v>8918.254000000001</v>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" s="3" t="n">
-        <v>44727</v>
-      </c>
-      <c r="B99" t="n">
-        <v>8932.42</v>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" s="3" t="n">
-        <v>44734</v>
-      </c>
-      <c r="B100" t="n">
-        <v>8934.346</v>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" s="3" t="n">
-        <v>44741</v>
-      </c>
-      <c r="B101" t="n">
-        <v>8913.553</v>
-      </c>
-    </row>
-    <row r="102">
-      <c r="A102" s="3" t="n">
-        <v>44748</v>
-      </c>
-      <c r="B102" t="n">
-        <v>8891.851000000001</v>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" s="3" t="n">
-        <v>44755</v>
-      </c>
-      <c r="B103" t="n">
-        <v>8895.867</v>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" s="3" t="n">
-        <v>44762</v>
-      </c>
-      <c r="B104" t="n">
-        <v>8899.213</v>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" s="3" t="n">
-        <v>44769</v>
-      </c>
-      <c r="B105" t="n">
-        <v>8890.004000000001</v>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" s="3" t="n">
-        <v>44776</v>
-      </c>
-      <c r="B106" t="n">
-        <v>8874.620000000001</v>
-      </c>
-    </row>
-    <row r="107">
-      <c r="A107" s="3" t="n">
-        <v>44783</v>
-      </c>
-      <c r="B107" t="n">
-        <v>8879.138000000001</v>
-      </c>
-    </row>
-    <row r="108">
-      <c r="A108" s="3" t="n">
-        <v>44790</v>
-      </c>
-      <c r="B108" t="n">
-        <v>8849.762000000001</v>
-      </c>
-    </row>
-    <row r="109">
-      <c r="A109" s="3" t="n">
-        <v>44797</v>
-      </c>
-      <c r="B109" t="n">
-        <v>8851.436</v>
-      </c>
-    </row>
-    <row r="110">
-      <c r="A110" s="3" t="n">
-        <v>44804</v>
-      </c>
-      <c r="B110" t="n">
-        <v>8826.093000000001</v>
-      </c>
-    </row>
-    <row r="111">
-      <c r="A111" s="3" t="n">
-        <v>44811</v>
-      </c>
-      <c r="B111" t="n">
-        <v>8822.401</v>
-      </c>
-    </row>
-    <row r="112">
-      <c r="A112" s="3" t="n">
-        <v>44818</v>
-      </c>
-      <c r="B112" t="n">
-        <v>8832.759</v>
-      </c>
-    </row>
-    <row r="113">
-      <c r="A113" s="3" t="n">
-        <v>44825</v>
-      </c>
-      <c r="B113" t="n">
-        <v>8816.802</v>
-      </c>
-    </row>
-    <row r="114">
-      <c r="A114" s="3" t="n">
-        <v>44832</v>
-      </c>
-      <c r="B114" t="n">
-        <v>8795.566999999999</v>
-      </c>
-    </row>
-    <row r="115">
-      <c r="A115" s="3" t="n">
-        <v>44839</v>
-      </c>
-      <c r="B115" t="n">
-        <v>8759.053</v>
-      </c>
-    </row>
-    <row r="116">
-      <c r="A116" s="3" t="n">
-        <v>44846</v>
-      </c>
-      <c r="B116" t="n">
-        <v>8758.968999999999</v>
-      </c>
-    </row>
-    <row r="117">
-      <c r="A117" s="3" t="n">
-        <v>44853</v>
-      </c>
-      <c r="B117" t="n">
-        <v>8743.922</v>
-      </c>
-    </row>
-    <row r="118">
-      <c r="A118" s="3" t="n">
-        <v>44860</v>
-      </c>
-      <c r="B118" t="n">
-        <v>8723.09</v>
-      </c>
-    </row>
-    <row r="119">
-      <c r="A119" s="3" t="n">
-        <v>44867</v>
-      </c>
-      <c r="B119" t="n">
-        <v>8676.870000000001</v>
-      </c>
-    </row>
-    <row r="120">
-      <c r="A120" s="3" t="n">
-        <v>44874</v>
-      </c>
-      <c r="B120" t="n">
-        <v>8678.886</v>
-      </c>
-    </row>
-    <row r="121">
-      <c r="A121" s="3" t="n">
-        <v>44881</v>
-      </c>
-      <c r="B121" t="n">
-        <v>8625.620000000001</v>
-      </c>
-    </row>
-    <row r="122">
-      <c r="A122" s="3" t="n">
-        <v>44888</v>
-      </c>
-      <c r="B122" t="n">
-        <v>8621.389999999999</v>
-      </c>
-    </row>
-    <row r="123">
-      <c r="A123" s="3" t="n">
-        <v>44895</v>
-      </c>
-      <c r="B123" t="n">
-        <v>8584.575999999999</v>
-      </c>
-    </row>
-    <row r="124">
-      <c r="A124" s="3" t="n">
-        <v>44902</v>
-      </c>
-      <c r="B124" t="n">
-        <v>8582.735000000001</v>
-      </c>
-    </row>
-    <row r="125">
-      <c r="A125" s="3" t="n">
-        <v>44909</v>
-      </c>
-      <c r="B125" t="n">
-        <v>8583.413</v>
-      </c>
-    </row>
-    <row r="126">
-      <c r="A126" s="3" t="n">
-        <v>44916</v>
-      </c>
-      <c r="B126" t="n">
-        <v>8564.411</v>
-      </c>
-    </row>
-    <row r="127">
-      <c r="A127" s="3" t="n">
-        <v>44923</v>
-      </c>
-      <c r="B127" t="n">
-        <v>8551.169</v>
-      </c>
-    </row>
-    <row r="128">
-      <c r="A128" s="3" t="n">
-        <v>44930</v>
-      </c>
-      <c r="B128" t="n">
-        <v>8507.429</v>
-      </c>
-    </row>
-    <row r="129">
-      <c r="A129" s="3" t="n">
-        <v>44937</v>
-      </c>
-      <c r="B129" t="n">
-        <v>8508.587</v>
-      </c>
-    </row>
-    <row r="130">
-      <c r="A130" s="3" t="n">
-        <v>44944</v>
-      </c>
-      <c r="B130" t="n">
-        <v>8489.039000000001</v>
-      </c>
-    </row>
-    <row r="131">
-      <c r="A131" s="3" t="n">
-        <v>44951</v>
-      </c>
-      <c r="B131" t="n">
-        <v>8470.557000000001</v>
-      </c>
-    </row>
-    <row r="132">
-      <c r="A132" s="3" t="n">
-        <v>44958</v>
-      </c>
-      <c r="B132" t="n">
-        <v>8433.610000000001</v>
+        <v>8298.312</v>
       </c>
     </row>
   </sheetData>
@@ -1548,7 +1236,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2023-02-07</t>
+          <t>2023-07-09</t>
         </is>
       </c>
     </row>
@@ -1560,7 +1248,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2023-02-07</t>
+          <t>2023-07-09</t>
         </is>
       </c>
     </row>
@@ -1596,7 +1284,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2023-02-01</t>
+          <t>2023-07-05</t>
         </is>
       </c>
     </row>
@@ -1632,7 +1320,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Millions of U.S. Dollars</t>
+          <t>Billions of U.S. Dollars</t>
         </is>
       </c>
     </row>
@@ -1644,7 +1332,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Mil. of U.S. $</t>
+          <t>Bil. of U.S. $</t>
         </is>
       </c>
     </row>
@@ -1680,7 +1368,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2023-02-02 15:35:25-06</t>
+          <t>2023-07-06 15:33:42-05</t>
         </is>
       </c>
     </row>
@@ -1691,7 +1379,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding quandl as a new data source. Improved API key management.
</commit_message>
<xml_diff>
--- a/NetLiquidity/FRED_Data/WALCL.xlsx
+++ b/NetLiquidity/FRED_Data/WALCL.xlsx
@@ -2,8 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Data" sheetId="1" state="visible" r:id="rId1"/>
@@ -19,18 +20,10 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <b val="1"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
@@ -47,27 +40,12 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -88,12 +66,12 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -458,7 +436,7 @@
   </sheetPr>
   <dimension ref="A1:B120"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -477,7 +455,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="n">
+      <c r="A2" s="3" t="n">
         <v>44440</v>
       </c>
       <c r="B2" t="n">
@@ -485,7 +463,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="n">
+      <c r="A3" s="3" t="n">
         <v>44447</v>
       </c>
       <c r="B3" t="n">
@@ -493,7 +471,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="n">
+      <c r="A4" s="3" t="n">
         <v>44454</v>
       </c>
       <c r="B4" t="n">
@@ -501,7 +479,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="n">
+      <c r="A5" s="3" t="n">
         <v>44461</v>
       </c>
       <c r="B5" t="n">
@@ -509,7 +487,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="2" t="n">
+      <c r="A6" s="3" t="n">
         <v>44468</v>
       </c>
       <c r="B6" t="n">
@@ -517,7 +495,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="2" t="n">
+      <c r="A7" s="3" t="n">
         <v>44475</v>
       </c>
       <c r="B7" t="n">
@@ -525,7 +503,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="2" t="n">
+      <c r="A8" s="3" t="n">
         <v>44482</v>
       </c>
       <c r="B8" t="n">
@@ -533,7 +511,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="2" t="n">
+      <c r="A9" s="3" t="n">
         <v>44489</v>
       </c>
       <c r="B9" t="n">
@@ -541,7 +519,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="2" t="n">
+      <c r="A10" s="3" t="n">
         <v>44496</v>
       </c>
       <c r="B10" t="n">
@@ -549,7 +527,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="2" t="n">
+      <c r="A11" s="3" t="n">
         <v>44503</v>
       </c>
       <c r="B11" t="n">
@@ -557,7 +535,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="2" t="n">
+      <c r="A12" s="3" t="n">
         <v>44510</v>
       </c>
       <c r="B12" t="n">
@@ -565,7 +543,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="2" t="n">
+      <c r="A13" s="3" t="n">
         <v>44517</v>
       </c>
       <c r="B13" t="n">
@@ -573,7 +551,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="2" t="n">
+      <c r="A14" s="3" t="n">
         <v>44524</v>
       </c>
       <c r="B14" t="n">
@@ -581,7 +559,7 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="2" t="n">
+      <c r="A15" s="3" t="n">
         <v>44531</v>
       </c>
       <c r="B15" t="n">
@@ -589,7 +567,7 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="2" t="n">
+      <c r="A16" s="3" t="n">
         <v>44538</v>
       </c>
       <c r="B16" t="n">
@@ -597,7 +575,7 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="2" t="n">
+      <c r="A17" s="3" t="n">
         <v>44545</v>
       </c>
       <c r="B17" t="n">
@@ -605,7 +583,7 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="2" t="n">
+      <c r="A18" s="3" t="n">
         <v>44552</v>
       </c>
       <c r="B18" t="n">
@@ -613,7 +591,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="2" t="n">
+      <c r="A19" s="3" t="n">
         <v>44559</v>
       </c>
       <c r="B19" t="n">
@@ -621,7 +599,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="2" t="n">
+      <c r="A20" s="3" t="n">
         <v>44566</v>
       </c>
       <c r="B20" t="n">
@@ -629,7 +607,7 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="2" t="n">
+      <c r="A21" s="3" t="n">
         <v>44573</v>
       </c>
       <c r="B21" t="n">
@@ -637,7 +615,7 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="2" t="n">
+      <c r="A22" s="3" t="n">
         <v>44580</v>
       </c>
       <c r="B22" t="n">
@@ -645,7 +623,7 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="2" t="n">
+      <c r="A23" s="3" t="n">
         <v>44587</v>
       </c>
       <c r="B23" t="n">
@@ -653,7 +631,7 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="2" t="n">
+      <c r="A24" s="3" t="n">
         <v>44594</v>
       </c>
       <c r="B24" t="n">
@@ -661,7 +639,7 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="2" t="n">
+      <c r="A25" s="3" t="n">
         <v>44601</v>
       </c>
       <c r="B25" t="n">
@@ -669,7 +647,7 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="2" t="n">
+      <c r="A26" s="3" t="n">
         <v>44608</v>
       </c>
       <c r="B26" t="n">
@@ -677,7 +655,7 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="2" t="n">
+      <c r="A27" s="3" t="n">
         <v>44615</v>
       </c>
       <c r="B27" t="n">
@@ -685,7 +663,7 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="2" t="n">
+      <c r="A28" s="3" t="n">
         <v>44622</v>
       </c>
       <c r="B28" t="n">
@@ -693,7 +671,7 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="2" t="n">
+      <c r="A29" s="3" t="n">
         <v>44629</v>
       </c>
       <c r="B29" t="n">
@@ -701,7 +679,7 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="2" t="n">
+      <c r="A30" s="3" t="n">
         <v>44636</v>
       </c>
       <c r="B30" t="n">
@@ -709,7 +687,7 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="2" t="n">
+      <c r="A31" s="3" t="n">
         <v>44643</v>
       </c>
       <c r="B31" t="n">
@@ -717,7 +695,7 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="2" t="n">
+      <c r="A32" s="3" t="n">
         <v>44650</v>
       </c>
       <c r="B32" t="n">
@@ -725,7 +703,7 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="2" t="n">
+      <c r="A33" s="3" t="n">
         <v>44657</v>
       </c>
       <c r="B33" t="n">
@@ -733,7 +711,7 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="2" t="n">
+      <c r="A34" s="3" t="n">
         <v>44664</v>
       </c>
       <c r="B34" t="n">
@@ -741,7 +719,7 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="2" t="n">
+      <c r="A35" s="3" t="n">
         <v>44671</v>
       </c>
       <c r="B35" t="n">
@@ -749,7 +727,7 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="2" t="n">
+      <c r="A36" s="3" t="n">
         <v>44678</v>
       </c>
       <c r="B36" t="n">
@@ -757,7 +735,7 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="2" t="n">
+      <c r="A37" s="3" t="n">
         <v>44685</v>
       </c>
       <c r="B37" t="n">
@@ -765,7 +743,7 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="2" t="n">
+      <c r="A38" s="3" t="n">
         <v>44692</v>
       </c>
       <c r="B38" t="n">
@@ -773,7 +751,7 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="2" t="n">
+      <c r="A39" s="3" t="n">
         <v>44699</v>
       </c>
       <c r="B39" t="n">
@@ -781,7 +759,7 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="2" t="n">
+      <c r="A40" s="3" t="n">
         <v>44706</v>
       </c>
       <c r="B40" t="n">
@@ -789,7 +767,7 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="2" t="n">
+      <c r="A41" s="3" t="n">
         <v>44713</v>
       </c>
       <c r="B41" t="n">
@@ -797,7 +775,7 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="2" t="n">
+      <c r="A42" s="3" t="n">
         <v>44720</v>
       </c>
       <c r="B42" t="n">
@@ -805,7 +783,7 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="2" t="n">
+      <c r="A43" s="3" t="n">
         <v>44727</v>
       </c>
       <c r="B43" t="n">
@@ -813,7 +791,7 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="2" t="n">
+      <c r="A44" s="3" t="n">
         <v>44734</v>
       </c>
       <c r="B44" t="n">
@@ -821,7 +799,7 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="2" t="n">
+      <c r="A45" s="3" t="n">
         <v>44741</v>
       </c>
       <c r="B45" t="n">
@@ -829,7 +807,7 @@
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="2" t="n">
+      <c r="A46" s="3" t="n">
         <v>44748</v>
       </c>
       <c r="B46" t="n">
@@ -837,7 +815,7 @@
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="2" t="n">
+      <c r="A47" s="3" t="n">
         <v>44755</v>
       </c>
       <c r="B47" t="n">
@@ -845,7 +823,7 @@
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="2" t="n">
+      <c r="A48" s="3" t="n">
         <v>44762</v>
       </c>
       <c r="B48" t="n">
@@ -853,7 +831,7 @@
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="2" t="n">
+      <c r="A49" s="3" t="n">
         <v>44769</v>
       </c>
       <c r="B49" t="n">
@@ -861,7 +839,7 @@
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="2" t="n">
+      <c r="A50" s="3" t="n">
         <v>44776</v>
       </c>
       <c r="B50" t="n">
@@ -869,7 +847,7 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="2" t="n">
+      <c r="A51" s="3" t="n">
         <v>44783</v>
       </c>
       <c r="B51" t="n">
@@ -877,7 +855,7 @@
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="2" t="n">
+      <c r="A52" s="3" t="n">
         <v>44790</v>
       </c>
       <c r="B52" t="n">
@@ -885,7 +863,7 @@
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="2" t="n">
+      <c r="A53" s="3" t="n">
         <v>44797</v>
       </c>
       <c r="B53" t="n">
@@ -893,7 +871,7 @@
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="2" t="n">
+      <c r="A54" s="3" t="n">
         <v>44804</v>
       </c>
       <c r="B54" t="n">
@@ -901,7 +879,7 @@
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="2" t="n">
+      <c r="A55" s="3" t="n">
         <v>44811</v>
       </c>
       <c r="B55" t="n">
@@ -909,7 +887,7 @@
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="2" t="n">
+      <c r="A56" s="3" t="n">
         <v>44818</v>
       </c>
       <c r="B56" t="n">
@@ -917,7 +895,7 @@
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="2" t="n">
+      <c r="A57" s="3" t="n">
         <v>44825</v>
       </c>
       <c r="B57" t="n">
@@ -925,7 +903,7 @@
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="2" t="n">
+      <c r="A58" s="3" t="n">
         <v>44832</v>
       </c>
       <c r="B58" t="n">
@@ -933,7 +911,7 @@
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="2" t="n">
+      <c r="A59" s="3" t="n">
         <v>44839</v>
       </c>
       <c r="B59" t="n">
@@ -941,7 +919,7 @@
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="2" t="n">
+      <c r="A60" s="3" t="n">
         <v>44846</v>
       </c>
       <c r="B60" t="n">
@@ -949,7 +927,7 @@
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="2" t="n">
+      <c r="A61" s="3" t="n">
         <v>44853</v>
       </c>
       <c r="B61" t="n">
@@ -957,7 +935,7 @@
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="2" t="n">
+      <c r="A62" s="3" t="n">
         <v>44860</v>
       </c>
       <c r="B62" t="n">
@@ -965,7 +943,7 @@
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="2" t="n">
+      <c r="A63" s="3" t="n">
         <v>44867</v>
       </c>
       <c r="B63" t="n">
@@ -973,7 +951,7 @@
       </c>
     </row>
     <row r="64">
-      <c r="A64" s="2" t="n">
+      <c r="A64" s="3" t="n">
         <v>44874</v>
       </c>
       <c r="B64" t="n">
@@ -981,7 +959,7 @@
       </c>
     </row>
     <row r="65">
-      <c r="A65" s="2" t="n">
+      <c r="A65" s="3" t="n">
         <v>44881</v>
       </c>
       <c r="B65" t="n">
@@ -989,7 +967,7 @@
       </c>
     </row>
     <row r="66">
-      <c r="A66" s="2" t="n">
+      <c r="A66" s="3" t="n">
         <v>44888</v>
       </c>
       <c r="B66" t="n">
@@ -997,7 +975,7 @@
       </c>
     </row>
     <row r="67">
-      <c r="A67" s="2" t="n">
+      <c r="A67" s="3" t="n">
         <v>44895</v>
       </c>
       <c r="B67" t="n">
@@ -1005,7 +983,7 @@
       </c>
     </row>
     <row r="68">
-      <c r="A68" s="2" t="n">
+      <c r="A68" s="3" t="n">
         <v>44902</v>
       </c>
       <c r="B68" t="n">
@@ -1013,7 +991,7 @@
       </c>
     </row>
     <row r="69">
-      <c r="A69" s="2" t="n">
+      <c r="A69" s="3" t="n">
         <v>44909</v>
       </c>
       <c r="B69" t="n">
@@ -1021,7 +999,7 @@
       </c>
     </row>
     <row r="70">
-      <c r="A70" s="2" t="n">
+      <c r="A70" s="3" t="n">
         <v>44916</v>
       </c>
       <c r="B70" t="n">
@@ -1029,7 +1007,7 @@
       </c>
     </row>
     <row r="71">
-      <c r="A71" s="2" t="n">
+      <c r="A71" s="3" t="n">
         <v>44923</v>
       </c>
       <c r="B71" t="n">
@@ -1037,7 +1015,7 @@
       </c>
     </row>
     <row r="72">
-      <c r="A72" s="2" t="n">
+      <c r="A72" s="3" t="n">
         <v>44930</v>
       </c>
       <c r="B72" t="n">
@@ -1045,7 +1023,7 @@
       </c>
     </row>
     <row r="73">
-      <c r="A73" s="2" t="n">
+      <c r="A73" s="3" t="n">
         <v>44937</v>
       </c>
       <c r="B73" t="n">
@@ -1053,7 +1031,7 @@
       </c>
     </row>
     <row r="74">
-      <c r="A74" s="2" t="n">
+      <c r="A74" s="3" t="n">
         <v>44944</v>
       </c>
       <c r="B74" t="n">
@@ -1061,7 +1039,7 @@
       </c>
     </row>
     <row r="75">
-      <c r="A75" s="2" t="n">
+      <c r="A75" s="3" t="n">
         <v>44951</v>
       </c>
       <c r="B75" t="n">
@@ -1069,7 +1047,7 @@
       </c>
     </row>
     <row r="76">
-      <c r="A76" s="2" t="n">
+      <c r="A76" s="3" t="n">
         <v>44958</v>
       </c>
       <c r="B76" t="n">
@@ -1077,7 +1055,7 @@
       </c>
     </row>
     <row r="77">
-      <c r="A77" s="2" t="n">
+      <c r="A77" s="3" t="n">
         <v>44965</v>
       </c>
       <c r="B77" t="n">
@@ -1085,7 +1063,7 @@
       </c>
     </row>
     <row r="78">
-      <c r="A78" s="2" t="n">
+      <c r="A78" s="3" t="n">
         <v>44972</v>
       </c>
       <c r="B78" t="n">
@@ -1093,7 +1071,7 @@
       </c>
     </row>
     <row r="79">
-      <c r="A79" s="2" t="n">
+      <c r="A79" s="3" t="n">
         <v>44979</v>
       </c>
       <c r="B79" t="n">
@@ -1101,7 +1079,7 @@
       </c>
     </row>
     <row r="80">
-      <c r="A80" s="2" t="n">
+      <c r="A80" s="3" t="n">
         <v>44986</v>
       </c>
       <c r="B80" t="n">
@@ -1109,7 +1087,7 @@
       </c>
     </row>
     <row r="81">
-      <c r="A81" s="2" t="n">
+      <c r="A81" s="3" t="n">
         <v>44993</v>
       </c>
       <c r="B81" t="n">
@@ -1117,7 +1095,7 @@
       </c>
     </row>
     <row r="82">
-      <c r="A82" s="2" t="n">
+      <c r="A82" s="3" t="n">
         <v>45000</v>
       </c>
       <c r="B82" t="n">
@@ -1125,7 +1103,7 @@
       </c>
     </row>
     <row r="83">
-      <c r="A83" s="2" t="n">
+      <c r="A83" s="3" t="n">
         <v>45007</v>
       </c>
       <c r="B83" t="n">
@@ -1133,7 +1111,7 @@
       </c>
     </row>
     <row r="84">
-      <c r="A84" s="2" t="n">
+      <c r="A84" s="3" t="n">
         <v>45014</v>
       </c>
       <c r="B84" t="n">
@@ -1141,7 +1119,7 @@
       </c>
     </row>
     <row r="85">
-      <c r="A85" s="2" t="n">
+      <c r="A85" s="3" t="n">
         <v>45021</v>
       </c>
       <c r="B85" t="n">
@@ -1149,7 +1127,7 @@
       </c>
     </row>
     <row r="86">
-      <c r="A86" s="2" t="n">
+      <c r="A86" s="3" t="n">
         <v>45028</v>
       </c>
       <c r="B86" t="n">
@@ -1157,7 +1135,7 @@
       </c>
     </row>
     <row r="87">
-      <c r="A87" s="2" t="n">
+      <c r="A87" s="3" t="n">
         <v>45035</v>
       </c>
       <c r="B87" t="n">
@@ -1165,7 +1143,7 @@
       </c>
     </row>
     <row r="88">
-      <c r="A88" s="2" t="n">
+      <c r="A88" s="3" t="n">
         <v>45042</v>
       </c>
       <c r="B88" t="n">
@@ -1173,7 +1151,7 @@
       </c>
     </row>
     <row r="89">
-      <c r="A89" s="2" t="n">
+      <c r="A89" s="3" t="n">
         <v>45049</v>
       </c>
       <c r="B89" t="n">
@@ -1181,7 +1159,7 @@
       </c>
     </row>
     <row r="90">
-      <c r="A90" s="2" t="n">
+      <c r="A90" s="3" t="n">
         <v>45056</v>
       </c>
       <c r="B90" t="n">
@@ -1189,7 +1167,7 @@
       </c>
     </row>
     <row r="91">
-      <c r="A91" s="2" t="n">
+      <c r="A91" s="3" t="n">
         <v>45063</v>
       </c>
       <c r="B91" t="n">
@@ -1197,7 +1175,7 @@
       </c>
     </row>
     <row r="92">
-      <c r="A92" s="2" t="n">
+      <c r="A92" s="3" t="n">
         <v>45070</v>
       </c>
       <c r="B92" t="n">
@@ -1205,7 +1183,7 @@
       </c>
     </row>
     <row r="93">
-      <c r="A93" s="2" t="n">
+      <c r="A93" s="3" t="n">
         <v>45077</v>
       </c>
       <c r="B93" t="n">
@@ -1213,7 +1191,7 @@
       </c>
     </row>
     <row r="94">
-      <c r="A94" s="2" t="n">
+      <c r="A94" s="3" t="n">
         <v>45084</v>
       </c>
       <c r="B94" t="n">
@@ -1221,7 +1199,7 @@
       </c>
     </row>
     <row r="95">
-      <c r="A95" s="2" t="n">
+      <c r="A95" s="3" t="n">
         <v>45091</v>
       </c>
       <c r="B95" t="n">
@@ -1229,7 +1207,7 @@
       </c>
     </row>
     <row r="96">
-      <c r="A96" s="2" t="n">
+      <c r="A96" s="3" t="n">
         <v>45098</v>
       </c>
       <c r="B96" t="n">
@@ -1237,7 +1215,7 @@
       </c>
     </row>
     <row r="97">
-      <c r="A97" s="2" t="n">
+      <c r="A97" s="3" t="n">
         <v>45105</v>
       </c>
       <c r="B97" t="n">
@@ -1245,7 +1223,7 @@
       </c>
     </row>
     <row r="98">
-      <c r="A98" s="2" t="n">
+      <c r="A98" s="3" t="n">
         <v>45112</v>
       </c>
       <c r="B98" t="n">
@@ -1253,7 +1231,7 @@
       </c>
     </row>
     <row r="99">
-      <c r="A99" s="2" t="n">
+      <c r="A99" s="3" t="n">
         <v>45119</v>
       </c>
       <c r="B99" t="n">
@@ -1261,7 +1239,7 @@
       </c>
     </row>
     <row r="100">
-      <c r="A100" s="2" t="n">
+      <c r="A100" s="3" t="n">
         <v>45126</v>
       </c>
       <c r="B100" t="n">
@@ -1269,7 +1247,7 @@
       </c>
     </row>
     <row r="101">
-      <c r="A101" s="2" t="n">
+      <c r="A101" s="3" t="n">
         <v>45133</v>
       </c>
       <c r="B101" t="n">
@@ -1277,7 +1255,7 @@
       </c>
     </row>
     <row r="102">
-      <c r="A102" s="2" t="n">
+      <c r="A102" s="3" t="n">
         <v>45140</v>
       </c>
       <c r="B102" t="n">
@@ -1285,7 +1263,7 @@
       </c>
     </row>
     <row r="103">
-      <c r="A103" s="2" t="n">
+      <c r="A103" s="3" t="n">
         <v>45147</v>
       </c>
       <c r="B103" t="n">
@@ -1293,7 +1271,7 @@
       </c>
     </row>
     <row r="104">
-      <c r="A104" s="2" t="n">
+      <c r="A104" s="3" t="n">
         <v>45154</v>
       </c>
       <c r="B104" t="n">
@@ -1301,7 +1279,7 @@
       </c>
     </row>
     <row r="105">
-      <c r="A105" s="2" t="n">
+      <c r="A105" s="3" t="n">
         <v>45161</v>
       </c>
       <c r="B105" t="n">
@@ -1309,7 +1287,7 @@
       </c>
     </row>
     <row r="106">
-      <c r="A106" s="2" t="n">
+      <c r="A106" s="3" t="n">
         <v>45168</v>
       </c>
       <c r="B106" t="n">
@@ -1317,7 +1295,7 @@
       </c>
     </row>
     <row r="107">
-      <c r="A107" s="2" t="n">
+      <c r="A107" s="3" t="n">
         <v>45175</v>
       </c>
       <c r="B107" t="n">
@@ -1325,7 +1303,7 @@
       </c>
     </row>
     <row r="108">
-      <c r="A108" s="2" t="n">
+      <c r="A108" s="3" t="n">
         <v>45182</v>
       </c>
       <c r="B108" t="n">
@@ -1333,7 +1311,7 @@
       </c>
     </row>
     <row r="109">
-      <c r="A109" s="2" t="n">
+      <c r="A109" s="3" t="n">
         <v>45189</v>
       </c>
       <c r="B109" t="n">
@@ -1341,7 +1319,7 @@
       </c>
     </row>
     <row r="110">
-      <c r="A110" s="2" t="n">
+      <c r="A110" s="3" t="n">
         <v>45196</v>
       </c>
       <c r="B110" t="n">
@@ -1349,7 +1327,7 @@
       </c>
     </row>
     <row r="111">
-      <c r="A111" s="2" t="n">
+      <c r="A111" s="3" t="n">
         <v>45203</v>
       </c>
       <c r="B111" t="n">
@@ -1357,7 +1335,7 @@
       </c>
     </row>
     <row r="112">
-      <c r="A112" s="2" t="n">
+      <c r="A112" s="3" t="n">
         <v>45210</v>
       </c>
       <c r="B112" t="n">
@@ -1365,7 +1343,7 @@
       </c>
     </row>
     <row r="113">
-      <c r="A113" s="2" t="n">
+      <c r="A113" s="3" t="n">
         <v>45217</v>
       </c>
       <c r="B113" t="n">
@@ -1373,7 +1351,7 @@
       </c>
     </row>
     <row r="114">
-      <c r="A114" s="2" t="n">
+      <c r="A114" s="3" t="n">
         <v>45224</v>
       </c>
       <c r="B114" t="n">
@@ -1381,7 +1359,7 @@
       </c>
     </row>
     <row r="115">
-      <c r="A115" s="2" t="n">
+      <c r="A115" s="3" t="n">
         <v>45231</v>
       </c>
       <c r="B115" t="n">
@@ -1389,7 +1367,7 @@
       </c>
     </row>
     <row r="116">
-      <c r="A116" s="2" t="n">
+      <c r="A116" s="3" t="n">
         <v>45238</v>
       </c>
       <c r="B116" t="n">
@@ -1397,7 +1375,7 @@
       </c>
     </row>
     <row r="117">
-      <c r="A117" s="2" t="n">
+      <c r="A117" s="3" t="n">
         <v>45245</v>
       </c>
       <c r="B117" t="n">
@@ -1405,7 +1383,7 @@
       </c>
     </row>
     <row r="118">
-      <c r="A118" s="2" t="n">
+      <c r="A118" s="3" t="n">
         <v>45252</v>
       </c>
       <c r="B118" t="n">
@@ -1413,7 +1391,7 @@
       </c>
     </row>
     <row r="119">
-      <c r="A119" s="2" t="n">
+      <c r="A119" s="3" t="n">
         <v>45259</v>
       </c>
       <c r="B119" t="n">
@@ -1421,7 +1399,7 @@
       </c>
     </row>
     <row r="120">
-      <c r="A120" s="2" t="n">
+      <c r="A120" s="3" t="n">
         <v>45266</v>
       </c>
       <c r="B120" t="n">
@@ -1429,7 +1407,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -1448,14 +1426,14 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="3" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>WALCL</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="inlineStr">
+      <c r="A2" s="1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
@@ -1467,31 +1445,31 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="inlineStr">
+      <c r="A3" s="1" t="inlineStr">
         <is>
           <t>realtime_start</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2023-12-08</t>
+          <t>2023-12-10</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="inlineStr">
+      <c r="A4" s="1" t="inlineStr">
         <is>
           <t>realtime_end</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2023-12-08</t>
+          <t>2023-12-10</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="3" t="inlineStr">
+      <c r="A5" s="1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
@@ -1503,7 +1481,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="3" t="inlineStr">
+      <c r="A6" s="1" t="inlineStr">
         <is>
           <t>observation_start</t>
         </is>
@@ -1515,7 +1493,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="3" t="inlineStr">
+      <c r="A7" s="1" t="inlineStr">
         <is>
           <t>observation_end</t>
         </is>
@@ -1527,7 +1505,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="3" t="inlineStr">
+      <c r="A8" s="1" t="inlineStr">
         <is>
           <t>frequency</t>
         </is>
@@ -1539,7 +1517,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="3" t="inlineStr">
+      <c r="A9" s="1" t="inlineStr">
         <is>
           <t>frequency_short</t>
         </is>
@@ -1551,7 +1529,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="3" t="inlineStr">
+      <c r="A10" s="1" t="inlineStr">
         <is>
           <t>units</t>
         </is>
@@ -1563,7 +1541,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="3" t="inlineStr">
+      <c r="A11" s="1" t="inlineStr">
         <is>
           <t>units_short</t>
         </is>
@@ -1575,7 +1553,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="3" t="inlineStr">
+      <c r="A12" s="1" t="inlineStr">
         <is>
           <t>seasonal_adjustment</t>
         </is>
@@ -1587,7 +1565,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="3" t="inlineStr">
+      <c r="A13" s="1" t="inlineStr">
         <is>
           <t>seasonal_adjustment_short</t>
         </is>
@@ -1599,7 +1577,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="3" t="inlineStr">
+      <c r="A14" s="1" t="inlineStr">
         <is>
           <t>last_updated</t>
         </is>
@@ -1611,13 +1589,13 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="3" t="inlineStr">
+      <c r="A15" s="1" t="inlineStr">
         <is>
           <t>popularity</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>